<commit_message>
get this stupid ass asignment out of my way
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -8510,7 +8510,7 @@
         <v>0.19309</v>
       </c>
       <c r="HD12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -12976,7 +12976,7 @@
         <v>-0.55237</v>
       </c>
       <c r="HD19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -13614,7 +13614,7 @@
         <v>0.38894</v>
       </c>
       <c r="HD20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -29564,7 +29564,7 @@
         <v>-0.43875</v>
       </c>
       <c r="HD45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -42324,7 +42324,7 @@
         <v>0.0020834</v>
       </c>
       <c r="HD65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -46790,7 +46790,7 @@
         <v>0.30346</v>
       </c>
       <c r="HD72" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">

</xml_diff>